<commit_message>
fix: correct typo in heading that broke XLS file chunking
</commit_message>
<xml_diff>
--- a/assets/default/files/_metadata.xlsx
+++ b/assets/default/files/_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charnould/GitHub/pierre/assets/pierre-ia.org/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charnould/GitHub/pierre/assets/default/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5F8ED-695D-184E-B73A-7F4F8411FBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BAF132-8A07-3F42-AD3E-AB8BF577BE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E5B0FB10-8797-D243-A0FA-6D923D5CC0EA}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>public</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>exemple.docx</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -714,13 +714,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -731,47 +731,47 @@
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -786,15 +786,15 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -809,15 +809,15 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
fix: modify `_metadata.xlsx` to align with new features
</commit_message>
<xml_diff>
--- a/assets/default/files/_metadata.xlsx
+++ b/assets/default/files/_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charnould/GitHub/pierre/assets/default/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BAF132-8A07-3F42-AD3E-AB8BF577BE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6723546E-73EA-1140-BD6C-E9E2CBE46E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E5B0FB10-8797-D243-A0FA-6D923D5CC0EA}"/>
   </bookViews>
@@ -39,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>private</t>
-  </si>
-  <si>
-    <t>public</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>true</t>
   </si>
@@ -106,46 +100,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> au nom du fichier uploadé. Respecter les espaces et la casse.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-Le contenu du fichier est-il </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>privé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ou </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>public</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ?</t>
     </r>
   </si>
   <si>
@@ -223,13 +177,63 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quels </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>profils</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ont accès au document ?
+Si plusieurs, les séparer d'une </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>virgule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>.
+Les profils sont ceux définis dans le fichier relatif aux utilisateurs.</t>
+    </r>
+  </si>
+  <si>
+    <t>agent_astreinte, cadre_astreinte</t>
+  </si>
+  <si>
+    <t>cadre_astreinte, agent_jour</t>
+  </si>
+  <si>
+    <t>agent_jour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +274,23 @@
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -329,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -355,10 +376,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
@@ -698,13 +722,14 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
-    <col min="2" max="3" width="18.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.83203125" style="1" customWidth="1"/>
@@ -714,67 +739,67 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -786,18 +811,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -809,18 +834,18 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -831,13 +856,10 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F997:F1675 D4:D1675" xr:uid="{49006576-7484-B84D-A51B-69FE1DA1041A}">
       <formula1>1</formula1>
       <formula2>10</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{2D33CDDD-82FD-DF49-92A6-98CA2408197D}">
-      <formula1>"private,public"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F996" xr:uid="{1B35C915-B844-3A4E-8381-4D4F9C183493}">
       <formula1>"true,false"</formula1>

</xml_diff>